<commit_message>
More strict validation of the setting file.
</commit_message>
<xml_diff>
--- a/app/_resources/default_krbiz_order_unified_row_names.xlsx
+++ b/app/_resources/default_krbiz_order_unified_row_names.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
-    <t>Platform Name</t>
-  </si>
-  <si>
-    <t>Header Row</t>
+    <t>PlatformName</t>
+  </si>
+  <si>
+    <t>HeaderRow</t>
   </si>
   <si>
     <t>order_id</t>
@@ -261,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -270,13 +270,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,19 +585,19 @@
   <cols>
     <col min="1" max="1" style="3" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="4" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="23.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="25.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="3" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="3" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="3" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="3" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="3" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="3" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="3" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="3" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="3" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="3" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="3" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -650,7 +647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -693,7 +690,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -734,7 +731,7 @@
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -775,7 +772,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -818,7 +815,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -859,7 +856,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
Update wadiz default option info row name.
</commit_message>
<xml_diff>
--- a/app/_resources/default_krbiz_order_unified_row_names.xlsx
+++ b/app/_resources/default_krbiz_order_unified_row_names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>PlatformName</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>주문 상품</t>
-  </si>
-  <si>
-    <t>주문 옵션</t>
   </si>
   <si>
     <t>주문 수량</t>
@@ -647,7 +644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -690,7 +687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -704,36 +701,36 @@
         <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -751,7 +748,7 @@
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>21</v>
@@ -762,19 +759,19 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -783,41 +780,41 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O5" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="1" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -841,66 +838,66 @@
         <v>21</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update wadiz default option info.
</commit_message>
<xml_diff>
--- a/app/_resources/default_krbiz_order_unified_row_names.xlsx
+++ b/app/_resources/default_krbiz_order_unified_row_names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
   <si>
     <t>PlatformName</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>주문 상품</t>
+  </si>
+  <si>
+    <t>주문 옵션</t>
   </si>
   <si>
     <t>주문 수량</t>
@@ -720,37 +723,37 @@
         <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -769,7 +772,7 @@
         <v>21</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>23</v>
@@ -780,11 +783,11 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>28</v>
@@ -792,7 +795,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
@@ -801,42 +804,42 @@
         <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -861,67 +864,67 @@
         <v>23</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="1" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>